<commit_message>
Added basic rules, added map layouts to cheat sheet, minor text changes in the bingo gen
</commit_message>
<xml_diff>
--- a/SMG2 Bingo Cheat Sheet.xlsx
+++ b/SMG2 Bingo Cheat Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joean\Desktop\SMG2 Bingo Mod Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joean\Documents\SMG2-Bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AF8D6-2D5B-4CE9-AE85-4993A1A02DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E0B603-1BDA-4706-8452-AAAFACB3799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05086300-188C-47C4-B5A4-86EFC405464C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Sky Station Galaxy</t>
   </si>
@@ -226,6 +226,9 @@
 The Banktoad appearance cutscene no longer plays and Banktoad never appears in normal gameplay. This is because Banktoad is banned in SMG2 Bingo.
 The Mailtoad appearance cutscene now plays after collecting 3 stars, but the actual Mailtoad does not spawn until the normal 13 stars. This is necessary to prevent a crash, and ultimately should have little effect on gameplay.
 The Star Board appearance cutscene has been changed to 4 stars (from 16). It appears properly for this cutscene and can be used from that point on.</t>
+  </si>
+  <si>
+    <t>World Map Layout</t>
   </si>
 </sst>
 </file>
@@ -293,6 +296,438 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7619</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEFEBD23-E98C-4ED1-9BE2-DBAC7870EBA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9204959" y="1472460"/>
+          <a:ext cx="4130041" cy="790679"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>8148</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5335</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609384</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89C38AD-D1EB-4480-AEA7-8FB388356EDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9205488" y="2565655"/>
+          <a:ext cx="4129296" cy="749045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>91439</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BEA4222-8225-40AF-AA9F-EBAA1830DDB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9204960" y="366946"/>
+          <a:ext cx="4130040" cy="821773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7619</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9662</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54D39C66-1775-41D8-9559-2A92AD0A8B2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9204959" y="3662958"/>
+          <a:ext cx="4139703" cy="771882"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114298</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0725E4A-49AB-4C94-8F86-969E12BDA36A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9204960" y="4759511"/>
+          <a:ext cx="4130040" cy="841187"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>6402</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F477B15F-DF67-424B-8596-01F3B25896C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9204960" y="5859780"/>
+          <a:ext cx="4136442" cy="769620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>5390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9170</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A72C2EE4-E9A4-470D-84A2-3A6A1C67E5EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9197340" y="6954830"/>
+          <a:ext cx="4146830" cy="901390"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B979F80C-8F78-4CCC-BFF1-0B91D2247A02}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,9 +1042,10 @@
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
     <col min="8" max="8" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -631,8 +1067,11 @@
       <c r="I1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +1094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -678,7 +1117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -701,7 +1140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -724,7 +1163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -747,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -770,7 +1209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,7 +1232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -816,7 +1255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -833,7 +1272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -850,7 +1289,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -867,7 +1306,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -884,7 +1323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -901,7 +1340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -918,7 +1357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1250,5 +1689,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removing midway star barriers, fixing jarry camera, reducing GGen barrier to 40, updating cheat sheet, minor goal changes, new zip file
</commit_message>
<xml_diff>
--- a/SMG2 Bingo Cheat Sheet.xlsx
+++ b/SMG2 Bingo Cheat Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joean\Documents\SMG2-Bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E0B603-1BDA-4706-8452-AAAFACB3799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13960A16-CA37-4F93-872E-1079E23D8A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05086300-188C-47C4-B5A4-86EFC405464C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Sky Station Galaxy</t>
   </si>
@@ -183,37 +183,7 @@
     <t>Star Requirement</t>
   </si>
   <si>
-    <t>World 1 (End)</t>
-  </si>
-  <si>
-    <t>World 6 (Throwback)</t>
-  </si>
-  <si>
-    <t>World 6 (Battle Belt)</t>
-  </si>
-  <si>
-    <t>World 6 (Portal)</t>
-  </si>
-  <si>
-    <t>World S (Rolling Coaster)</t>
-  </si>
-  <si>
     <t>World 6 (Galaxy Generator)</t>
-  </si>
-  <si>
-    <t>World S (Twisty Trials)</t>
-  </si>
-  <si>
-    <t>World S (Stone Cyclone)</t>
-  </si>
-  <si>
-    <t>World S (Boss Blitz)</t>
-  </si>
-  <si>
-    <t>World S (Flip Out)</t>
-  </si>
-  <si>
-    <t>World 1 (Middle)</t>
   </si>
   <si>
     <t>Galaxies with Comets</t>
@@ -229,6 +199,9 @@
   </si>
   <si>
     <t>World Map Layout</t>
+  </si>
+  <si>
+    <t>World 6 (World S Portal)</t>
   </si>
 </sst>
 </file>
@@ -425,67 +398,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1186</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91439</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BEA4222-8225-40AF-AA9F-EBAA1830DDB5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9204960" y="366946"/>
-          <a:ext cx="4130040" cy="821773"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>7619</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>5358</xdr:rowOff>
@@ -510,7 +422,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -571,7 +483,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -608,60 +520,87 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>7619</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>6402</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>605532</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F477B15F-DF67-424B-8596-01F3B25896C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60364B70-13F0-4B9F-8684-8CAFAC1F5933}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9204960" y="5859780"/>
-          <a:ext cx="4136442" cy="769620"/>
+          <a:off x="9204959" y="370059"/>
+          <a:ext cx="4125973" cy="879621"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>608658</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FBBCC19-8A07-490B-9244-7F61BA3D4174}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9204960" y="5859959"/>
+          <a:ext cx="4129098" cy="830401"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -670,59 +609,42 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>5390</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180897</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>9170</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>112093</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A72C2EE4-E9A4-470D-84A2-3A6A1C67E5EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB54E722-6261-41BE-81A4-EC9D97B820D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9197340" y="6954830"/>
-          <a:ext cx="4146830" cy="901390"/>
+          <a:off x="9197340" y="6947457"/>
+          <a:ext cx="4145280" cy="1211356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1030,7 +952,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,10 +969,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1068,7 +990,7 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1088,10 +1010,10 @@
         <v>150</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1111,10 +1033,10 @@
         <v>300</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1134,10 +1056,10 @@
         <v>400</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1157,10 +1079,10 @@
         <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I5">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1180,10 +1102,10 @@
         <v>550</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I6">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1203,10 +1125,10 @@
         <v>600</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I7">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1226,10 +1148,10 @@
         <v>600</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1248,12 +1170,6 @@
       <c r="F9">
         <v>3100</v>
       </c>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9">
-        <v>32</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1265,12 +1181,6 @@
       <c r="C10" s="1">
         <v>22</v>
       </c>
-      <c r="H10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10">
-        <v>35</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1282,12 +1192,6 @@
       <c r="C11" s="1">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11">
-        <v>45</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1299,12 +1203,6 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12">
-        <v>36</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1316,12 +1214,6 @@
       <c r="C13" s="1">
         <v>12</v>
       </c>
-      <c r="H13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13">
-        <v>37</v>
-      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1333,12 +1225,6 @@
       <c r="C14" s="1">
         <v>10</v>
       </c>
-      <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14">
-        <v>38</v>
-      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1350,12 +1236,6 @@
       <c r="C15" s="1">
         <v>31</v>
       </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15">
-        <v>39</v>
-      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1367,12 +1247,6 @@
       <c r="C16" s="1">
         <v>27</v>
       </c>
-      <c r="H16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16">
-        <v>40</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1418,7 +1292,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>

</xml_diff>

<commit_message>
Bingo gen overhaul to fix types, lowered hungry luma requirement again, new zip file
</commit_message>
<xml_diff>
--- a/SMG2 Bingo Cheat Sheet.xlsx
+++ b/SMG2 Bingo Cheat Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joean\Documents\SMG2-Bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13960A16-CA37-4F93-872E-1079E23D8A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD3C974-BE75-490C-84E3-34C8C78D1C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05086300-188C-47C4-B5A4-86EFC405464C}"/>
+    <workbookView xWindow="0" yWindow="2976" windowWidth="17280" windowHeight="8964" xr2:uid="{05086300-188C-47C4-B5A4-86EFC405464C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1030,7 @@
         <v>39</v>
       </c>
       <c r="F3">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H3" t="s">
         <v>39</v>
@@ -1053,7 +1053,7 @@
         <v>40</v>
       </c>
       <c r="F4">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="H4" t="s">
         <v>40</v>
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="F5">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -1099,7 +1099,7 @@
         <v>42</v>
       </c>
       <c r="F6">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -1122,7 +1122,7 @@
         <v>43</v>
       </c>
       <c r="F7">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="H7" t="s">
         <v>54</v>
@@ -1145,7 +1145,7 @@
         <v>44</v>
       </c>
       <c r="F8">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="H8" t="s">
         <v>49</v>
@@ -1168,7 +1168,7 @@
         <v>47</v>
       </c>
       <c r="F9">
-        <v>3100</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>